<commit_message>
Update to GUI and Small Python Update
Removes some unused python data in the FMR Crawler. Adds additional data display lines to the GUI. Adds the ability to filter by state to the GUI. Added more test data to test the new GUI features.
</commit_message>
<xml_diff>
--- a/Crawlers/FMR_Crawler_Test_Excel.xlsx
+++ b/Crawlers/FMR_Crawler_Test_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\221Project\SectionM8-Demo-Fall2025\Crawlers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39473C70-E3AF-404A-AF50-B50F6FE4B3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D82A86E-F4CA-42BF-9321-3E5831B7663B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMR_Crawler_Test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="41">
   <si>
     <t>fiscal_year</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Region 3</t>
   </si>
   <si>
-    <t>1BR</t>
-  </si>
-  <si>
     <t>40%</t>
   </si>
   <si>
@@ -136,10 +133,16 @@
     <t>ETL_001</t>
   </si>
   <si>
-    <t>2BR</t>
-  </si>
-  <si>
-    <t>3BR</t>
+    <t>Aston</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>Camden</t>
   </si>
 </sst>
 </file>
@@ -479,15 +482,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2025</v>
       </c>
@@ -589,20 +595,20 @@
       <c r="J2">
         <v>19406</v>
       </c>
-      <c r="K2" t="s">
-        <v>29</v>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1234</v>
       </c>
       <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
       </c>
       <c r="P2">
         <v>1.04</v>
@@ -614,22 +620,22 @@
         <v>84500</v>
       </c>
       <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>35</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>36</v>
       </c>
-      <c r="W2" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -658,22 +664,22 @@
         <v>28</v>
       </c>
       <c r="J3">
-        <v>19406</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
+        <v>19403</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
       </c>
       <c r="L3">
         <v>1500</v>
       </c>
       <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
       </c>
       <c r="P3">
         <v>1.04</v>
@@ -682,25 +688,25 @@
         <v>1</v>
       </c>
       <c r="R3">
-        <v>84500</v>
+        <v>85000</v>
       </c>
       <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>34</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>35</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>36</v>
       </c>
-      <c r="W3" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -729,22 +735,22 @@
         <v>28</v>
       </c>
       <c r="J4">
-        <v>19406</v>
-      </c>
-      <c r="K4" t="s">
-        <v>39</v>
+        <v>19402</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
       </c>
       <c r="L4">
         <v>1740</v>
       </c>
       <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
       </c>
       <c r="P4">
         <v>1.04</v>
@@ -753,22 +759,306 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>84500</v>
+        <v>84000</v>
       </c>
       <c r="S4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
         <v>33</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>34</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>35</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>36</v>
       </c>
-      <c r="W4" t="s">
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
+      </c>
+      <c r="E5">
+        <v>42091</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>37980</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5">
+        <v>19300</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1350</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <v>1.04</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>80000</v>
+      </c>
+      <c r="S5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>42091</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6">
+        <v>37980</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6">
+        <v>19302</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>1800</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6">
+        <v>1.04</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>96000</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>42091</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>37980</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7">
+        <v>19301</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>2300</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7">
+        <v>1.04</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>100000</v>
+      </c>
+      <c r="S7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>42091</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8">
+        <v>37980</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8">
+        <v>19301</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>3300</v>
+      </c>
+      <c r="M8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8">
+        <v>1.04</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>130000</v>
+      </c>
+      <c r="S8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>